<commit_message>
some updates in the documentation about IPS types and endpoints that correspond to in Hades
</commit_message>
<xml_diff>
--- a/New Terminals/IPS-LI-TMF (transactions saved).xlsx
+++ b/New Terminals/IPS-LI-TMF (transactions saved).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD3A1BE-2514-4724-AFBC-AF3FC8A3803D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB1C3EE-1C72-4AA6-A4FD-A6ADA1565151}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2AF06A-391B-40AD-9C34-9E017E47FE0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2AF06A-391B-40AD-9C34-9E017E47FE0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="134">
   <si>
     <t>TRABUF(TITYP).EQ.IVAL</t>
   </si>
@@ -226,9 +226,6 @@
     <t xml:space="preserve">0xDD Validação/Pagamento Prémio LI </t>
   </si>
   <si>
-    <t xml:space="preserve">0xD6 - Encomenda Jogo LI </t>
-  </si>
-  <si>
     <t xml:space="preserve">0xDC - Confirmação Receção Encomenda Jogo LI </t>
   </si>
   <si>
@@ -416,13 +413,34 @@
   </si>
   <si>
     <t xml:space="preserve">0xD2 Alteração de Estado da Caixa/Carton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xD6 - Encomenda de Maços de LI </t>
+  </si>
+  <si>
+    <t>Not used</t>
+  </si>
+  <si>
+    <t>Activação de Maço</t>
+  </si>
+  <si>
+    <t>{{host-hades}}/instant/validation</t>
+  </si>
+  <si>
+    <t>{{host-hades}}/instant/packStatusChange</t>
+  </si>
+  <si>
+    <t>{{host-hades}}/instant/cartonStatusChange</t>
+  </si>
+  <si>
+    <t>{{host-hades}}/instant/quotaReport</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,8 +462,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +500,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -489,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -540,9 +570,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -552,42 +618,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,37 +1163,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9357B7-F398-410C-BF75-8CC0928D0E2B}">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D18"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.26953125" customWidth="1"/>
-    <col min="7" max="7" width="50.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" customWidth="1"/>
-    <col min="11" max="11" width="13.08984375" customWidth="1"/>
-    <col min="13" max="13" width="7.26953125" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" customWidth="1"/>
-    <col min="16" max="16" width="92.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" customWidth="1"/>
+    <col min="7" max="7" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="16" max="16" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H1" s="5" t="s">
         <v>50</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K1" s="26"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>8</v>
       </c>
@@ -1169,103 +1203,103 @@
       <c r="I2" s="5">
         <v>2</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K2" s="26"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H3" s="5">
         <v>13</v>
       </c>
       <c r="I3" s="5">
         <v>3</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H4" s="5">
         <v>13</v>
       </c>
       <c r="I4" s="5">
         <v>6</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="18"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H5" s="5">
         <v>13</v>
       </c>
       <c r="I5" s="5">
         <v>7</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="18"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K5" s="26"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H6" s="5">
         <v>13</v>
       </c>
       <c r="I6" s="5">
         <v>8</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="18"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H7" s="5">
         <v>13</v>
       </c>
       <c r="I7" s="5">
         <v>12</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H8" s="5">
         <v>13</v>
       </c>
       <c r="I8" s="5">
         <v>13</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H9" s="5">
         <v>13</v>
       </c>
       <c r="I9" s="5">
         <v>14</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="18"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>2</v>
@@ -1285,12 +1319,12 @@
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="P11" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>0</v>
@@ -1298,7 +1332,7 @@
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
       <c r="E12" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>63</v>
@@ -1306,18 +1340,21 @@
       <c r="G12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="P12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>4</v>
@@ -1325,26 +1362,31 @@
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>129</v>
+      </c>
       <c r="G13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>6</v>
@@ -1352,28 +1394,31 @@
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>8</v>
@@ -1381,28 +1426,31 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>126</v>
+        <v>73</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>10</v>
@@ -1410,139 +1458,148 @@
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="8"/>
+        <v>74</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="G16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="P16" s="35"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="9"/>
+        <v>87</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="G17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="H17" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="P17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="P17" s="35"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
       <c r="E18" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
       <c r="P18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
       <c r="E19" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>122</v>
+        <v>77</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>121</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="P19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
       <c r="E20" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="G20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="P20" s="35"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>15</v>
@@ -1550,25 +1607,28 @@
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
       <c r="E21" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="G21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="P21" s="35"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>16</v>
@@ -1576,116 +1636,123 @@
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="E22" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>65</v>
+        <v>79</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
       <c r="P22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="P23" s="35"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="G24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="P24" s="35"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
       <c r="E25" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="G25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="P25" s="35"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="4" t="s">
@@ -1700,361 +1767,362 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P26" s="35"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="19" t="s">
         <v>49</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="H27" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
       <c r="P27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B28" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B29" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B30" s="19" t="s">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="25" t="s">
         <v>89</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>90</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
       <c r="F36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:17" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C38" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" t="s">
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="16" t="s">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q43" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="G44" s="22"/>
+      <c r="Q44" s="23"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="G45" s="22"/>
+      <c r="Q45" s="23"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="G46" s="22"/>
+      <c r="Q46" s="23"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="G47" s="22"/>
+      <c r="Q47" s="23"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
+      <c r="Q48" s="23"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
+      <c r="Q49" s="23"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
+      <c r="Q50" s="23"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="Q51" s="23"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="24"/>
+      <c r="Q52" s="23"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" s="24"/>
+      <c r="Q53" s="23"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="24"/>
+      <c r="Q54" s="23"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="24"/>
+      <c r="Q55" s="23"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="24"/>
+      <c r="Q56" s="23"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="24"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="24"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="24"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="24"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" s="24"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="24"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="22"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="22"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+    </row>
+    <row r="74" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="22"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
+      <c r="F90" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="22"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>113</v>
       </c>
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="18" t="s">
+      <c r="C96" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" s="22"/>
+      <c r="E96" s="22"/>
+      <c r="F96" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="18" t="s">
+    </row>
+    <row r="97" spans="2:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F97" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>115</v>
+      </c>
+      <c r="C101" s="22"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="22"/>
+      <c r="F101" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>100</v>
-      </c>
-      <c r="G40" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-      <c r="G41" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G43" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q43" s="29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A44" s="27"/>
-      <c r="G44" s="28"/>
-      <c r="Q44" s="29"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A45" s="27"/>
-      <c r="G45" s="28"/>
-      <c r="Q45" s="29"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A46" s="27"/>
-      <c r="G46" s="28"/>
-      <c r="Q46" s="29"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A47" s="27"/>
-      <c r="G47" s="28"/>
-      <c r="Q47" s="29"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="27"/>
-      <c r="Q48" s="29"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A49" s="27"/>
-      <c r="Q49" s="29"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A50" s="27"/>
-      <c r="Q50" s="29"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A51" s="27"/>
-      <c r="Q51" s="29"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A52" s="27"/>
-      <c r="Q52" s="29"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A53" s="27"/>
-      <c r="Q53" s="29"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A54" s="27"/>
-      <c r="Q54" s="29"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A55" s="27"/>
-      <c r="Q55" s="29"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A56" s="27"/>
-      <c r="Q56" s="29"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A57" s="27"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A58" s="27"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A59" s="27"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A60" s="27"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A62" s="27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A63" s="27"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A64" s="27"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="28"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="28"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="28"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="28"/>
-    </row>
-    <row r="74" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="28"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="28"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="28"/>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>108</v>
-      </c>
-      <c r="C90" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
-      <c r="F90" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F91" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F92" s="28"/>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F93" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B96" t="s">
-        <v>114</v>
-      </c>
-      <c r="C96" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F97" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F98" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B101" t="s">
+    </row>
+    <row r="102" spans="2:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F102" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F102" s="16" t="s">
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="F103" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E109">
         <v>20</v>
       </c>
       <c r="F109" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E110">
         <v>15</v>
       </c>
@@ -2064,51 +2132,6 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="G43:G47"/>
-    <mergeCell ref="Q43:Q56"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="A43:A60"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="H13:O13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="H14:O14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="H15:O15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="H16:N16"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="H22:N22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
@@ -2125,6 +2148,51 @@
     <mergeCell ref="H19:N19"/>
     <mergeCell ref="H20:N20"/>
     <mergeCell ref="H21:N21"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H22:N22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="H14:O14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="H15:O15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="H16:N16"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="H13:O13"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="A43:A60"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="Q43:Q56"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="F91:F92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>